<commit_message>
update kdr001 fix bug
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_V6.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_V6.xlsx
@@ -94,7 +94,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="71">
+  <borders count="74">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -589,6 +589,27 @@
       <left/>
       <right/>
       <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -630,7 +651,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1195,12 +1216,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="44" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="61" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="72" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="73" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1289,9 +1318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>282600</xdr:colOff>
+      <xdr:colOff>281520</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1301,7 +1330,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3768840" y="676080"/>
-          <a:ext cx="241200" cy="201600"/>
+          <a:ext cx="240120" cy="200520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1331,7 +1360,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W56"/>
+  <dimension ref="A1:W60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2696,54 +2725,154 @@
       <c r="A55" s="141"/>
       <c r="B55" s="141"/>
       <c r="C55" s="142"/>
-      <c r="D55" s="142"/>
-      <c r="E55" s="142"/>
-      <c r="F55" s="142"/>
-      <c r="G55" s="142"/>
-      <c r="H55" s="142"/>
-      <c r="I55" s="142"/>
-      <c r="J55" s="142"/>
-      <c r="K55" s="142"/>
-      <c r="L55" s="142"/>
-      <c r="M55" s="142"/>
-      <c r="N55" s="142"/>
-      <c r="O55" s="142"/>
-      <c r="P55" s="142"/>
-      <c r="Q55" s="142"/>
-      <c r="R55" s="142"/>
-      <c r="S55" s="142"/>
-      <c r="T55" s="142"/>
-      <c r="U55" s="142"/>
-      <c r="V55" s="142"/>
-      <c r="W55" s="142"/>
+      <c r="D55" s="143"/>
+      <c r="E55" s="143"/>
+      <c r="F55" s="143"/>
+      <c r="G55" s="143"/>
+      <c r="H55" s="143"/>
+      <c r="I55" s="143"/>
+      <c r="J55" s="143"/>
+      <c r="K55" s="143"/>
+      <c r="L55" s="143"/>
+      <c r="M55" s="143"/>
+      <c r="N55" s="143"/>
+      <c r="O55" s="143"/>
+      <c r="P55" s="143"/>
+      <c r="Q55" s="143"/>
+      <c r="R55" s="143"/>
+      <c r="S55" s="143"/>
+      <c r="T55" s="143"/>
+      <c r="U55" s="143"/>
+      <c r="V55" s="143"/>
+      <c r="W55" s="144"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="141"/>
       <c r="B56" s="141"/>
       <c r="C56" s="142"/>
-      <c r="D56" s="142"/>
-      <c r="E56" s="142"/>
-      <c r="F56" s="142"/>
-      <c r="G56" s="142"/>
-      <c r="H56" s="142"/>
-      <c r="I56" s="142"/>
-      <c r="J56" s="142"/>
-      <c r="K56" s="142"/>
-      <c r="L56" s="142"/>
-      <c r="M56" s="142"/>
-      <c r="N56" s="142"/>
-      <c r="O56" s="142"/>
-      <c r="P56" s="142"/>
-      <c r="Q56" s="142"/>
-      <c r="R56" s="142"/>
-      <c r="S56" s="142"/>
-      <c r="T56" s="142"/>
-      <c r="U56" s="142"/>
-      <c r="V56" s="142"/>
-      <c r="W56" s="142"/>
+      <c r="D56" s="143"/>
+      <c r="E56" s="143"/>
+      <c r="F56" s="143"/>
+      <c r="G56" s="143"/>
+      <c r="H56" s="143"/>
+      <c r="I56" s="143"/>
+      <c r="J56" s="143"/>
+      <c r="K56" s="143"/>
+      <c r="L56" s="143"/>
+      <c r="M56" s="143"/>
+      <c r="N56" s="143"/>
+      <c r="O56" s="143"/>
+      <c r="P56" s="143"/>
+      <c r="Q56" s="143"/>
+      <c r="R56" s="143"/>
+      <c r="S56" s="143"/>
+      <c r="T56" s="143"/>
+      <c r="U56" s="143"/>
+      <c r="V56" s="143"/>
+      <c r="W56" s="144"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="141"/>
+      <c r="B57" s="141"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="143"/>
+      <c r="E57" s="143"/>
+      <c r="F57" s="143"/>
+      <c r="G57" s="143"/>
+      <c r="H57" s="143"/>
+      <c r="I57" s="143"/>
+      <c r="J57" s="143"/>
+      <c r="K57" s="143"/>
+      <c r="L57" s="143"/>
+      <c r="M57" s="143"/>
+      <c r="N57" s="143"/>
+      <c r="O57" s="143"/>
+      <c r="P57" s="143"/>
+      <c r="Q57" s="143"/>
+      <c r="R57" s="143"/>
+      <c r="S57" s="143"/>
+      <c r="T57" s="143"/>
+      <c r="U57" s="143"/>
+      <c r="V57" s="143"/>
+      <c r="W57" s="144"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="141"/>
+      <c r="B58" s="141"/>
+      <c r="C58" s="142"/>
+      <c r="D58" s="143"/>
+      <c r="E58" s="143"/>
+      <c r="F58" s="143"/>
+      <c r="G58" s="143"/>
+      <c r="H58" s="143"/>
+      <c r="I58" s="143"/>
+      <c r="J58" s="143"/>
+      <c r="K58" s="143"/>
+      <c r="L58" s="143"/>
+      <c r="M58" s="143"/>
+      <c r="N58" s="143"/>
+      <c r="O58" s="143"/>
+      <c r="P58" s="143"/>
+      <c r="Q58" s="143"/>
+      <c r="R58" s="143"/>
+      <c r="S58" s="143"/>
+      <c r="T58" s="143"/>
+      <c r="U58" s="143"/>
+      <c r="V58" s="143"/>
+      <c r="W58" s="144"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="141"/>
+      <c r="B59" s="141"/>
+      <c r="C59" s="142"/>
+      <c r="D59" s="143"/>
+      <c r="E59" s="143"/>
+      <c r="F59" s="143"/>
+      <c r="G59" s="143"/>
+      <c r="H59" s="143"/>
+      <c r="I59" s="143"/>
+      <c r="J59" s="143"/>
+      <c r="K59" s="143"/>
+      <c r="L59" s="143"/>
+      <c r="M59" s="143"/>
+      <c r="N59" s="143"/>
+      <c r="O59" s="143"/>
+      <c r="P59" s="143"/>
+      <c r="Q59" s="143"/>
+      <c r="R59" s="143"/>
+      <c r="S59" s="143"/>
+      <c r="T59" s="143"/>
+      <c r="U59" s="143"/>
+      <c r="V59" s="143"/>
+      <c r="W59" s="144"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="141"/>
+      <c r="B60" s="141"/>
+      <c r="C60" s="142"/>
+      <c r="D60" s="143"/>
+      <c r="E60" s="143"/>
+      <c r="F60" s="143"/>
+      <c r="G60" s="143"/>
+      <c r="H60" s="143"/>
+      <c r="I60" s="143"/>
+      <c r="J60" s="143"/>
+      <c r="K60" s="143"/>
+      <c r="L60" s="143"/>
+      <c r="M60" s="143"/>
+      <c r="N60" s="143"/>
+      <c r="O60" s="143"/>
+      <c r="P60" s="143"/>
+      <c r="Q60" s="143"/>
+      <c r="R60" s="143"/>
+      <c r="S60" s="143"/>
+      <c r="T60" s="143"/>
+      <c r="U60" s="143"/>
+      <c r="V60" s="143"/>
+      <c r="W60" s="144"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="A2:W2"/>
     <mergeCell ref="E4:I4"/>
@@ -2765,8 +2894,7 @@
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A55:B56"/>
-    <mergeCell ref="C55:W56"/>
+    <mergeCell ref="A55:B60"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.5" bottom="1.5" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>